<commit_message>
-updated TVims lab_2 -updated electro lab_2
</commit_message>
<xml_diff>
--- a/ЭЛЕКТРОНИКА/labs/lab2/ОТЧЁТ/lab2.xlsx
+++ b/ЭЛЕКТРОНИКА/labs/lab2/ОТЧЁТ/lab2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20730" windowHeight="9270" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20736" windowHeight="9276" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>нагузочная прямая????????</t>
-  </si>
-  <si>
-    <t>нагрузочную прямую???</t>
   </si>
   <si>
     <t>Iб,мкА</t>
@@ -65,9 +62,6 @@
     <t>Iс, мА</t>
   </si>
   <si>
-    <t>Uз2 = 2,,2 В</t>
-  </si>
-  <si>
     <t>Uз1 = 2,0 В</t>
   </si>
   <si>
@@ -86,15 +80,22 @@
     <t>Ес = 6 В</t>
   </si>
   <si>
-    <t>Iб0 = 6 мкА</t>
+    <t>Iбн1 = 6,3 мкА</t>
+  </si>
+  <si>
+    <t>Iбн2 = 3 мкА</t>
+  </si>
+  <si>
+    <t>Uз2 = 2,2 В</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -442,11 +443,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -471,14 +481,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,7 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -568,6 +584,29 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3370954799927603E-2"/>
+                  <c:y val="-4.7501034176059116E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -575,7 +614,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numLit>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>\О\с\н\о\в\н\о\й</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -584,10 +623,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Лист1!$D$5:$L$5</c:f>
+                <c:f>Лист1!$D$5:$M$5</c:f>
                 <c:numCache>
-                  <c:formatCode>Основной</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -604,15 +643,18 @@
                     <c:v>3</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>6.3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>10</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>18</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>26</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>33</c:v>
                   </c:pt>
                 </c:numCache>
@@ -620,6 +662,7 @@
             </c:minus>
             <c:spPr>
               <a:ln>
+                <a:noFill/>
                 <a:prstDash val="dash"/>
               </a:ln>
             </c:spPr>
@@ -631,7 +674,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numLit>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>\О\с\н\о\в\н\о\й</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -640,10 +683,10 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Лист1!$D$4:$L$4</c:f>
+                <c:f>Лист1!$D$4:$M$4</c:f>
                 <c:numCache>
-                  <c:formatCode>Основной</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
@@ -660,15 +703,18 @@
                     <c:v>0.6</c:v>
                   </c:pt>
                   <c:pt idx="5">
+                    <c:v>0.66</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
                     <c:v>0.7</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>0.8</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>0.9</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>1</c:v>
                   </c:pt>
                 </c:numCache>
@@ -676,16 +722,17 @@
             </c:minus>
             <c:spPr>
               <a:ln>
+                <a:noFill/>
                 <a:prstDash val="dash"/>
               </a:ln>
             </c:spPr>
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$D$4:$L$4</c:f>
+              <c:f>Лист1!$D$4:$M$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -702,15 +749,18 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -718,10 +768,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$D$5:$L$5</c:f>
+              <c:f>Лист1!$D$5:$M$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -738,15 +788,18 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
@@ -762,11 +815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92539136"/>
-        <c:axId val="92541312"/>
+        <c:axId val="254170240"/>
+        <c:axId val="254172160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92539136"/>
+        <c:axId val="254170240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,16 +868,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92541312"/>
+        <c:crossAx val="254172160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92541312"/>
+        <c:axId val="254172160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,11 +919,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92539136"/>
+        <c:crossAx val="254170240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -939,14 +992,19 @@
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Iб0</c:v>
+            <c:v>Iбр</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -954,7 +1012,7 @@
             <c:numRef>
               <c:f>Лист2!$E$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -982,11 +1040,11 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$E$6:$K$6</c:f>
+              <c:f>Лист2!$E$2:$K$2</c:f>
               <c:numCache>
-                <c:formatCode>0,00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="Основной">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1010,7 +1068,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -1025,7 +1083,7 @@
             <c:numRef>
               <c:f>Лист2!$E$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1053,9 +1111,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$E$7:$K$7</c:f>
+              <c:f>Лист2!$E$6:$K$6</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1081,7 +1139,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1096,7 +1154,7 @@
             <c:numRef>
               <c:f>Лист2!$E$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1124,9 +1182,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$E$8:$K$8</c:f>
+              <c:f>Лист2!$E$7:$K$7</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1152,7 +1210,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1167,7 +1225,7 @@
             <c:numRef>
               <c:f>Лист2!$E$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1195,9 +1253,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$E$9:$K$9</c:f>
+              <c:f>Лист2!$E$8:$K$8</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1223,7 +1281,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1238,7 +1296,7 @@
             <c:numRef>
               <c:f>Лист2!$E$5:$K$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1266,9 +1324,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$E$10:$K$10</c:f>
+              <c:f>Лист2!$E$9:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1294,7 +1352,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1307,10 +1365,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="star"/>
-              <c:size val="4"/>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dLbls>
@@ -1355,9 +1409,9 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист2!$N$5:$N$7</c:f>
+              <c:f>Лист2!$N$2:$N$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
@@ -1373,9 +1427,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист2!$O$5:$O$7</c:f>
+              <c:f>Лист2!$O$2:$O$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1389,7 +1443,83 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Iнб2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист2!$E$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист2!$E$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1399,16 +1529,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92599040"/>
-        <c:axId val="92600960"/>
+        <c:axId val="254681856"/>
+        <c:axId val="254683776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92599040"/>
+        <c:axId val="254681856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1419,8 +1551,12 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>U</a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Ек,</a:t>
+                  <a:t>кэ,</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
@@ -1434,28 +1570,29 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.8460564306231193"/>
-              <c:y val="0.79159664922124251"/>
+              <c:x val="0.78443036651522324"/>
+              <c:y val="0.81589026928315289"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92600960"/>
+        <c:crossAx val="254683776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92600960"/>
+        <c:axId val="254683776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1491,18 +1628,27 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92599040"/>
+        <c:crossAx val="254681856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76216189331052142"/>
+          <c:y val="0.28210553767362617"/>
+          <c:w val="0.23783810668947855"/>
+          <c:h val="0.5125163232826121"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1582,7 +1728,7 @@
             <c:numRef>
               <c:f>Лист3!$D$6:$I$6</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1609,7 +1755,7 @@
             <c:numRef>
               <c:f>Лист3!$D$7:$I$7</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1640,6 +1786,11 @@
           <c:tx>
             <c:v>Ек2</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1647,7 +1798,7 @@
             <c:numRef>
               <c:f>Лист3!$D$6:$I$6</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1674,7 +1825,7 @@
             <c:numRef>
               <c:f>Лист3!$D$8:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1707,11 +1858,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105202048"/>
-        <c:axId val="105203968"/>
+        <c:axId val="254726528"/>
+        <c:axId val="254728448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105202048"/>
+        <c:axId val="254726528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,16 +1903,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105203968"/>
+        <c:crossAx val="254728448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105203968"/>
+        <c:axId val="254728448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1805,11 +1956,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105202048"/>
+        <c:crossAx val="254726528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1878,7 +2029,7 @@
           <c:yMode val="edge"/>
           <c:x val="9.6335739282589664E-2"/>
           <c:y val="0.20881017012237774"/>
-          <c:w val="0.71537248468941395"/>
+          <c:w val="0.66666624054039625"/>
           <c:h val="0.70952184766635218"/>
         </c:manualLayout>
       </c:layout>
@@ -1898,7 +2049,7 @@
             <c:numRef>
               <c:f>Лист4!$D$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1928,7 +2079,7 @@
             <c:numRef>
               <c:f>Лист4!$D$5:$J$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1969,7 +2120,7 @@
             <c:numRef>
               <c:f>Лист4!$D$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1999,7 +2150,7 @@
             <c:numRef>
               <c:f>Лист4!$D$6:$J$6</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2040,7 +2191,7 @@
             <c:numRef>
               <c:f>Лист4!$D$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2070,7 +2221,7 @@
             <c:numRef>
               <c:f>Лист4!$D$7:$J$7</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2111,7 +2262,7 @@
             <c:numRef>
               <c:f>Лист4!$D$4:$J$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2141,7 +2292,7 @@
             <c:numRef>
               <c:f>Лист4!$D$8:$J$8</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2193,7 +2344,7 @@
             <c:numRef>
               <c:f>Лист4!$F$12:$F$14</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2211,7 +2362,7 @@
             <c:numRef>
               <c:f>Лист4!$E$12:$E$14</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>2.8</c:v>
@@ -2221,6 +2372,82 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Uзн</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист4!$D$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист4!$D$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4500000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2235,16 +2462,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105715200"/>
-        <c:axId val="105717120"/>
+        <c:axId val="254952960"/>
+        <c:axId val="254954880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105715200"/>
+        <c:axId val="254952960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2255,8 +2484,12 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>U</a:t>
+                </a:r>
+                <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Ес,</a:t>
+                  <a:t>си,</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
@@ -2270,28 +2503,29 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.82230664916885388"/>
-              <c:y val="0.86241225959224532"/>
+              <c:x val="0.77765924365356831"/>
+              <c:y val="0.87382792404393506"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105717120"/>
+        <c:crossAx val="254954880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105717120"/>
+        <c:axId val="254954880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2327,18 +2561,27 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105715200"/>
+        <c:crossAx val="254952960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77497861338939411"/>
+          <c:y val="0.19629662803944822"/>
+          <c:w val="0.21143118158654101"/>
+          <c:h val="0.62995158691333841"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2427,7 +2670,7 @@
             <c:numRef>
               <c:f>Лист5!$E$4:$N$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2466,7 +2709,7 @@
             <c:numRef>
               <c:f>Лист5!$E$5:$N$5</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2516,7 +2759,7 @@
             <c:numRef>
               <c:f>Лист5!$E$4:$N$4</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2555,7 +2798,7 @@
             <c:numRef>
               <c:f>Лист5!$E$6:$N$6</c:f>
               <c:numCache>
-                <c:formatCode>Основной</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2600,11 +2843,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105122048"/>
-        <c:axId val="105169280"/>
+        <c:axId val="255079552"/>
+        <c:axId val="255081472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105122048"/>
+        <c:axId val="255079552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2640,16 +2883,16 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105169280"/>
+        <c:crossAx val="255081472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105169280"/>
+        <c:axId val="255081472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,11 +2934,11 @@
           </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="Основной" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105122048"/>
+        <c:crossAx val="255079552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2727,7 +2970,7 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -2756,16 +2999,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>518904</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>77443</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27248</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>176503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>588065</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>20293</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>96409</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119353</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2792,13 +3035,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>165735</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>470535</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -2827,13 +3070,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
+      <xdr:colOff>164124</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
@@ -3179,20 +3422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:L9"/>
+  <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3211,22 +3454,25 @@
       <c r="H4" s="3">
         <v>0.6</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="28">
+        <v>0.66</v>
+      </c>
+      <c r="J4" s="3">
         <v>0.7</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>0.8</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>0.9</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -3243,34 +3489,43 @@
       <c r="H5" s="7">
         <v>3</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="28">
+        <v>6.3</v>
+      </c>
+      <c r="J5" s="7">
         <v>10</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="7">
         <v>18</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>26</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="8">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="J7" s="10">
-        <f>(0.1/8)/(7*10^-6)</f>
-        <v>1785.7142857142858</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="K7" s="10">
+        <f>(0.0775)/(7*10^-6)</f>
+        <v>11071.428571428571</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="M9">
         <f>(7/2.5)/100</f>
         <v>2.7999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <f>(0.7-0.6)/((10-3)*10^-3)</f>
+        <v>14.285714285714283</v>
       </c>
     </row>
   </sheetData>
@@ -3281,27 +3536,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:O32"/>
+  <dimension ref="B1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C1" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <f>1.075-0.44</f>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="G1">
+        <f t="shared" ref="G1:K1" si="0">1.075-0.44</f>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>0.63500000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25">
+        <f>6.3*10^-3*220</f>
+        <v>1.3860000000000001</v>
+      </c>
+      <c r="G2" s="25">
+        <f>6.3*10^-3*220</f>
+        <v>1.3860000000000001</v>
+      </c>
+      <c r="H2" s="25">
+        <f>6.3*10^-3*220.5</f>
+        <v>1.3891500000000001</v>
+      </c>
+      <c r="I2" s="25">
+        <f>6.3*10^-3*220.7</f>
+        <v>1.3904099999999999</v>
+      </c>
+      <c r="J2" s="25">
+        <f>6.3*10^-3*220.9</f>
+        <v>1.39167</v>
+      </c>
+      <c r="K2" s="25">
+        <f>6.3*10^-3*221</f>
+        <v>1.3923000000000001</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <f>N2/2</f>
+        <v>3.5</v>
+      </c>
+      <c r="O4">
+        <f>O3/2</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="20"/>
       <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>2</v>
       </c>
       <c r="G5" s="7">
@@ -3319,224 +3662,192 @@
       <c r="K5" s="8">
         <v>11</v>
       </c>
-      <c r="N5">
-        <v>7</v>
-      </c>
-      <c r="O5">
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5">
+      <c r="F6" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J6" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K6" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="23">
         <v>0</v>
       </c>
-      <c r="F6" s="30">
-        <f>6.3*10^-3*220</f>
-        <v>1.3860000000000001</v>
-      </c>
-      <c r="G6" s="30">
-        <f>6.3*10^-3*220</f>
-        <v>1.3860000000000001</v>
-      </c>
-      <c r="H6" s="30">
-        <f>6.3*10^-3*220.5</f>
-        <v>1.3891500000000001</v>
-      </c>
-      <c r="I6" s="30">
-        <f>6.3*10^-3*220.7</f>
-        <v>1.3904099999999999</v>
-      </c>
-      <c r="J6" s="30">
-        <f>6.3*10^-3*220.9</f>
-        <v>1.39167</v>
-      </c>
-      <c r="K6" s="30">
-        <f>6.3*10^-3*221</f>
-        <v>1.3923000000000001</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
+      <c r="F7" s="11">
+        <v>2.7</v>
+      </c>
+      <c r="G7" s="11">
+        <v>2.75</v>
+      </c>
+      <c r="H7" s="11">
+        <v>2.77</v>
+      </c>
+      <c r="I7" s="11">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="22">
-        <v>0</v>
-      </c>
-      <c r="F7" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G7" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H7" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I7" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J7" s="18">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K7" s="19">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N7">
-        <f>N5/2</f>
-        <v>3.5</v>
-      </c>
-      <c r="O7">
-        <f>O6/2</f>
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J7" s="11">
+        <v>2.81</v>
+      </c>
+      <c r="K7" s="13">
+        <v>2.81</v>
+      </c>
+      <c r="P7">
+        <f>((F2*10^-3)^2)*2.5*10^3</f>
+        <v>4.8024900000000004E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="23">
         <v>0</v>
       </c>
       <c r="F8" s="11">
-        <v>2.7</v>
+        <v>4.41</v>
       </c>
       <c r="G8" s="11">
-        <v>2.75</v>
+        <v>4.42</v>
       </c>
       <c r="H8" s="11">
-        <v>2.77</v>
+        <v>4.42</v>
       </c>
       <c r="I8" s="11">
-        <v>2.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J8" s="11">
-        <v>2.81</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K8" s="13">
-        <v>2.81</v>
-      </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="12" t="s">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="23">
+      <c r="D9" s="31"/>
+      <c r="E9" s="21">
         <v>0</v>
       </c>
-      <c r="F9" s="11">
-        <v>4.41</v>
-      </c>
-      <c r="G9" s="11">
-        <v>4.42</v>
-      </c>
-      <c r="H9" s="11">
-        <v>4.42</v>
-      </c>
-      <c r="I9" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J9" s="11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K9" s="13">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="21">
-        <v>0</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="F9" s="15">
         <v>5</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G9" s="15">
         <v>5.05</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H9" s="15">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I9" s="15">
         <v>5.15</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J9" s="15">
         <v>5.2</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K9" s="16">
         <v>5.4</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>((5.5 - 3.5))/((0.6-1.39) )</f>
+        <v>-2.5316455696202533</v>
+      </c>
+      <c r="C12">
+        <f>((1.4-0.63)*10^-3)/((6.3-3)*10^-6 )</f>
+        <v>233.33333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="C15">
         <f>7*10^-3*220</f>
         <v>1.54</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C21">
-        <v>5</v>
+        <v>4.41</v>
       </c>
       <c r="D21">
-        <v>5.05</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C22">
-        <v>4.41</v>
+        <v>2.75</v>
       </c>
       <c r="D22">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C23">
-        <v>2.75</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D23">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C24">
-        <v>2.2000000000000002</v>
+        <v>1.075</v>
       </c>
       <c r="D24">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <v>1.075</v>
-      </c>
-      <c r="D25">
         <v>1.05</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
         <v>2</v>
+      </c>
+      <c r="L31">
+        <f>7-1.39*(10^(-3))*2.5*10^3</f>
+        <v>3.5250000000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D6:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3547,17 +3858,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="20"/>
-      <c r="C6" s="26" t="s">
-        <v>10</v>
+      <c r="C6" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -3578,12 +3889,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="22">
         <v>0</v>
@@ -3604,11 +3915,11 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="28"/>
+        <v>10</v>
+      </c>
+      <c r="C8" s="33"/>
       <c r="D8" s="21">
         <v>0</v>
       </c>
@@ -3628,7 +3939,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D12">
         <f>((I7-H7)*10^-3)/((I6-H6)*10^-6)</f>
         <v>219.99999999999994</v>
@@ -3645,22 +3956,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J17"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>2.25</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1.35</v>
+      </c>
+      <c r="F2">
+        <f>E$2+$D$1</f>
+        <v>1.37</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:J2" si="0">F$2+$D$1</f>
+        <v>1.3900000000000001</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1.4100000000000001</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>1.4300000000000002</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>1.4500000000000002</v>
+      </c>
+      <c r="L2">
+        <f>((5.2-3.5))/((2.2-2.25))</f>
+        <v>-34.000000000000128</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20"/>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
@@ -3684,12 +4035,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="27" t="s">
         <v>14</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="22">
         <v>0</v>
@@ -3713,11 +4064,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="29"/>
+        <v>22</v>
+      </c>
+      <c r="C6" s="34"/>
       <c r="D6" s="23">
         <v>0</v>
       </c>
@@ -3740,11 +4091,11 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="29"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="34"/>
       <c r="D7" s="23">
         <v>0</v>
       </c>
@@ -3767,11 +4118,11 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="28"/>
+        <v>15</v>
+      </c>
+      <c r="C8" s="33"/>
       <c r="D8" s="21">
         <v>0</v>
       </c>
@@ -3794,7 +4145,15 @@
         <v>5.21</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="C12">
         <f>((F6-E6)/4) +E6</f>
         <v>0.6875</v>
@@ -3806,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>0</v>
       </c>
@@ -3814,7 +4173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="E14">
         <f>E12/2</f>
         <v>1.4</v>
@@ -3824,9 +4183,36 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="17" spans="5:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E17" s="9" t="s">
-        <v>3</v>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>3.8*1.35</f>
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>4.95</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>((1.7)*10^-3)/0.2</f>
+        <v>8.4999999999999989E-3</v>
+      </c>
+      <c r="D21">
+        <f>C21*2.3+$E$6</f>
+        <v>0.69955000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3841,19 +4227,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:N6"/>
+  <dimension ref="C1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="I1">
+        <f>((J5-I5)*10^-3)/(J4-I4)</f>
+        <v>9.9999999999999915E-3</v>
+      </c>
+    </row>
     <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="20"/>
-      <c r="D4" s="26" t="s">
-        <v>19</v>
+      <c r="D4" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
@@ -3886,12 +4278,12 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="22">
         <v>0</v>
@@ -3924,11 +4316,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="28"/>
+        <v>19</v>
+      </c>
+      <c r="D6" s="33"/>
       <c r="E6" s="21">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-added TViMS lab5 \n -rework TViMS lab4
</commit_message>
<xml_diff>
--- a/ЭЛЕКТРОНИКА/labs/lab2/ОТЧЁТ/lab2.xlsx
+++ b/ЭЛЕКТРОНИКА/labs/lab2/ОТЧЁТ/lab2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="122" windowWidth="20731" windowHeight="9278"/>
+    <workbookView xWindow="249" yWindow="118" windowWidth="20736" windowHeight="9281" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -815,11 +815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266167424"/>
-        <c:axId val="266169344"/>
+        <c:axId val="262386432"/>
+        <c:axId val="262388352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266167424"/>
+        <c:axId val="262386432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,12 +872,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266169344"/>
+        <c:crossAx val="262388352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266169344"/>
+        <c:axId val="262388352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266167424"/>
+        <c:crossAx val="262386432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -975,6 +975,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -991,7 +992,7 @@
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="5"/>
@@ -1067,7 +1068,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -1138,7 +1139,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1209,7 +1210,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1280,7 +1281,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1351,7 +1352,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1442,7 +1443,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1518,7 +1519,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1528,11 +1529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266908416"/>
-        <c:axId val="266910336"/>
+        <c:axId val="263324032"/>
+        <c:axId val="263325952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266908416"/>
+        <c:axId val="263324032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,12 +1580,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266910336"/>
+        <c:crossAx val="263325952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266910336"/>
+        <c:axId val="263325952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +1632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266908416"/>
+        <c:crossAx val="263324032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1644,8 +1645,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.76216189331052142"/>
           <c:y val="0.28210553767362617"/>
-          <c:w val="0.23783810668947855"/>
-          <c:h val="0.5125163232826121"/>
+          <c:w val="0.21827263102150815"/>
+          <c:h val="0.52193863636363635"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1856,11 +1857,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267252096"/>
-        <c:axId val="267254016"/>
+        <c:axId val="263471104"/>
+        <c:axId val="263473024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267252096"/>
+        <c:axId val="263471104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,12 +1906,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267254016"/>
+        <c:crossAx val="263473024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267254016"/>
+        <c:axId val="263473024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267252096"/>
+        <c:crossAx val="263471104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2458,11 +2459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267437952"/>
-        <c:axId val="267444224"/>
+        <c:axId val="263519616"/>
+        <c:axId val="263525888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267437952"/>
+        <c:axId val="263519616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,12 +2510,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267444224"/>
+        <c:crossAx val="263525888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267444224"/>
+        <c:axId val="263525888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2561,7 +2562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267437952"/>
+        <c:crossAx val="263519616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2839,11 +2840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267592832"/>
-        <c:axId val="267594752"/>
+        <c:axId val="263092864"/>
+        <c:axId val="263095040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267592832"/>
+        <c:axId val="263092864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,12 +2884,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267594752"/>
+        <c:crossAx val="263095040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267594752"/>
+        <c:axId val="263095040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2934,14 +2935,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267592832"/>
+        <c:crossAx val="263092864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3420,18 +3420,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" ht="14.95" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:13" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" ht="14.9" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -3501,24 +3501,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K7" s="10">
         <f>(0.0775)/(7*10^-6)</f>
         <v>11071.428571428571</v>
       </c>
     </row>
-    <row r="9" spans="3:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M9">
         <f>(7/2.5)/100</f>
         <v>2.7999999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="3:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="L16">
         <f>(0.7-0.6)/((10-3)*10^-3)</f>
         <v>14.285714285714283</v>
@@ -3534,16 +3534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C1" s="27" t="s">
         <v>21</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C2" s="27" t="s">
         <v>20</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="N3">
         <v>0</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="14.95" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="14.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N4">
         <f>N2/2</f>
         <v>3.5</v>
@@ -3632,7 +3632,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="20"/>
       <c r="D5" s="8" t="s">
         <v>1</v>
@@ -3659,7 +3659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C6" s="17" t="s">
         <v>5</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>4.8024900000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>((5.5 - 3.5))/((0.6-1.39) )</f>
         <v>-2.5316455696202533</v>
@@ -3783,16 +3783,16 @@
         <v>233.33333333333334</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E14" s="26"/>
     </row>
-    <row r="15" spans="2:16" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>7*10^-3*220</f>
         <v>1.54</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>5</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="21" spans="3:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>4.41</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>4.42</v>
       </c>
     </row>
-    <row r="22" spans="3:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2.75</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="23" spans="3:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>2.2000000000000002</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="24" spans="3:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>1.075</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>2</v>
       </c>
@@ -3858,10 +3858,10 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="2:9" ht="15.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:9" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="15.9" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="20"/>
       <c r="C6" s="24" t="s">
         <v>9</v>
@@ -3885,7 +3885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="14.9" x14ac:dyDescent="0.25">
       <c r="D12">
         <f>((I7-H7)*10^-3)/((I6-H6)*10^-6)</f>
         <v>219.99999999999994</v>
@@ -3958,17 +3958,17 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>2.25</v>
       </c>
@@ -4003,8 +4003,8 @@
         <v>-34.000000000000128</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="14.9" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20"/>
       <c r="C4" s="8" t="s">
         <v>12</v>
@@ -4031,7 +4031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>5.21</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="H10">
         <v>5</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="C12">
         <f>((F6-E6)/4) +E6</f>
         <v>0.6875</v>
@@ -4161,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>0</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="14.9" x14ac:dyDescent="0.25">
       <c r="E14">
         <f>E12/2</f>
         <v>1.4</v>
@@ -4179,7 +4179,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="G16">
         <f>3.8*1.35</f>
         <v>5.13</v>
@@ -4191,17 +4191,17 @@
       </c>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.68</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C21">
         <f>((1.7)*10^-3)/0.2</f>
         <v>8.4999999999999989E-3</v>
@@ -4229,16 +4229,16 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="3:14" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I1">
         <f>((J5-I5)*10^-3)/(J4-I4)</f>
         <v>9.9999999999999915E-3</v>
       </c>
     </row>
-    <row r="3" spans="3:14" ht="15.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:14" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" ht="15.9" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="20"/>
       <c r="D4" s="24" t="s">
         <v>17</v>
@@ -4274,7 +4274,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
         <v>18</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:14" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="14" t="s">
         <v>19</v>
       </c>

</xml_diff>